<commit_message>
Update read excel file and test data
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestData.xlsx
+++ b/src/test/resources/data/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://everisgroup-my.sharepoint.com/personal/Thomas_Schultz_emeal_nttdata_com/Documents/10 proj/Seat/VAP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\Selenium_Java\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{623FA20A-A91B-459E-A83F-B3ED387C23C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77B3DD08-B444-4E5E-8AE0-C9D8E67142E1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF31236-75BB-4371-A188-EE6689B5CD71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2565" yWindow="2250" windowWidth="21900" windowHeight="13050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11220" uniqueCount="9159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11221" uniqueCount="9160">
   <si>
     <t>used</t>
   </si>
@@ -27513,6 +27511,9 @@
   </si>
   <si>
     <t>Duong</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -27963,7 +27964,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -28053,7 +28054,9 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
+      <c r="A2" s="8" t="s">
+        <v>9159</v>
+      </c>
       <c r="B2" s="8">
         <v>1300</v>
       </c>

</xml_diff>

<commit_message>
Update new lead creation steps
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestData.xlsx
+++ b/src/test/resources/data/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\Selenium_Java\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ntpduong\Project\Selenium_Java\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF31236-75BB-4371-A188-EE6689B5CD71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B92CF8E-551B-4812-B732-27DB172FCE52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2565" yWindow="2250" windowWidth="21900" windowHeight="13050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11221" uniqueCount="9160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11222" uniqueCount="9160">
   <si>
     <t>used</t>
   </si>
@@ -27964,7 +27964,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -28113,7 +28113,9 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
+      <c r="A3" s="5" t="s">
+        <v>9159</v>
+      </c>
       <c r="B3" s="5">
         <v>1301</v>
       </c>

</xml_diff>